<commit_message>
Quero Morrer T3 A / B
GRÁFICOS DE RESIDUOS COM BARRAS DE INCERTEZA
</commit_message>
<xml_diff>
--- a/016/T3A/T3A.xlsx
+++ b/016/T3A/T3A.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\Desktop\faculdade\2º Ano\2ºS\LABS\LABSFISICAII\016\T3A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F6C0DF-E388-45C6-9A82-B32BC2CD79B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6E6080-737D-4BC3-8698-16CDC6AF055D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Varrimento Inicial " sheetId="3" r:id="rId1"/>
@@ -2161,6 +2161,116 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Coeficiente de Absorção #1'!$M$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>1.0000000000000001E-5</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Coeficiente de Absorção #1'!$M$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>1.0000000000000001E-5</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Coeficiente de Absorção #1'!$G$16:$G$20</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>4.2372881355932204E-7</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.1363636363636364E-6</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.5000000000000002E-6</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>7.1428571428571427E-6</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1.6666666666666667E-5</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Coeficiente de Absorção #1'!$G$16:$G$20</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>4.2372881355932204E-7</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.1363636363636364E-6</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.5000000000000002E-6</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>7.1428571428571427E-6</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1.6666666666666667E-5</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>'Coeficiente de Absorção #1'!$C$16:$C$23</c:f>
@@ -3462,6 +3572,116 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Coeficiente de Absorção #2'!$M$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>1.0000000000000001E-5</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Coeficiente de Absorção #2'!$M$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>1.0000000000000001E-5</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Coeficiente de Absorção #2'!$G$16:$G$20</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>4.3859649122807023E-6</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.2500000000000001E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3.1250000000000001E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>8.3333333333333331E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1.6666666666666666E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Coeficiente de Absorção #2'!$G$16:$G$20</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>4.3859649122807023E-6</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.2500000000000001E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3.1250000000000001E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>8.3333333333333331E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1.6666666666666666E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>'Coeficiente de Absorção #2'!$C$16:$C$23</c:f>
@@ -4759,6 +4979,116 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Coeficiente de Absorção #3'!$M$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>1.0000000000000001E-5</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Coeficiente de Absorção #3'!$M$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>1.0000000000000001E-5</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Coeficiente de Absorção #3'!$G$16:$G$20</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>4.8543689320388348E-6</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.0416666666666666E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.7777777777777779E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>8.3333333333333331E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1.25E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Coeficiente de Absorção #3'!$G$16:$G$20</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>4.8543689320388348E-6</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.0416666666666666E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.7777777777777779E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>8.3333333333333331E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1.25E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>'Coeficiente de Absorção #3'!$C$16:$C$23</c:f>
@@ -6056,6 +6386,116 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Coeficiente de Absorção #4'!$M$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>1.0000000000000001E-5</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Coeficiente de Absorção #4'!$M$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>1.0000000000000001E-5</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Coeficiente de Absorção #4'!$G$16:$G$20</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>4.0983606557377053E-6</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.1904761904761907E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.7777777777777779E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>8.3333333333333331E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1.6666666666666666E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Coeficiente de Absorção #4'!$G$16:$G$20</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>4.0983606557377053E-6</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.1904761904761907E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.7777777777777779E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>8.3333333333333331E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1.6666666666666666E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>'Coeficiente de Absorção #4'!$C$16:$C$23</c:f>
@@ -7486,6 +7926,116 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Coeficiente de Absorção #5'!$M$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>1.0000000000000001E-5</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Coeficiente de Absorção #5'!$M$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>1.0000000000000001E-5</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Coeficiente de Absorção #5'!$G$16:$G$20</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>4.0983606557377051E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.0638297872340425E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.0833333333333336E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.05</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.25</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Coeficiente de Absorção #5'!$G$16:$G$20</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>4.0983606557377051E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.0638297872340425E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.0833333333333336E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.05</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.25</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>'Coeficiente de Absorção #5'!$C$16:$C$23</c:f>
@@ -7839,8 +8389,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.17698538109201409"/>
-          <c:y val="0.67175300062846299"/>
+          <c:x val="0.17955988197839243"/>
+          <c:y val="0.6846329949574923"/>
           <c:w val="0.30174890603086413"/>
           <c:h val="7.2674902617583748E-2"/>
         </c:manualLayout>
@@ -9107,6 +9657,308 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Varrimento Inicial '!$I$9:$I$27</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="19"/>
+                  <c:pt idx="0">
+                    <c:v>1.0857362047581294E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.6858896380650357E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>7.2382413650541968E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>6.204206884332169E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>5.4286810237906471E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4.8254942433694642E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4.3429448190325179E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>3.9481316536659248E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>3.6191206825270984E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>3.3407267838711675E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>3.1021034421660845E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>2.8952965460216784E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>2.7143405118953235E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>2.5546734229603049E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>2.4127471216847321E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>2.2857604310697464E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>2.1714724095162589E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>2.0680689614440562E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>1.9740658268329624E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Varrimento Inicial '!$I$9:$I$27</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="19"/>
+                  <c:pt idx="0">
+                    <c:v>1.0857362047581294E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.6858896380650357E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>7.2382413650541968E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>6.204206884332169E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>5.4286810237906471E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4.8254942433694642E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4.3429448190325179E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>3.9481316536659248E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>3.6191206825270984E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>3.3407267838711675E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>3.1021034421660845E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>2.8952965460216784E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>2.7143405118953235E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>2.5546734229603049E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>2.4127471216847321E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>2.2857604310697464E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>2.1714724095162589E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>2.0680689614440562E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>1.9740658268329624E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Varrimento Inicial '!$K$9:$K$27</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="19"/>
+                  <c:pt idx="0">
+                    <c:v>6.9376115320008271E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.0147067334188125E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.4286002694185914E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1.9048003592247886E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2.4675822835412031E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>3.1021034421660845E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>3.8776293027076048E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>4.5239008531588727E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>5.4286810237906471E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>6.031867804211831E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>6.7858512797383086E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>7.7552586054152096E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>9.0478017063177455E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>1.0857362047581294E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>1.0857362047581294E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>1.2063735608423662E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>1.3571702559476617E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>1.3571702559476617E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>1.8095603412635491E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Varrimento Inicial '!$K$9:$K$27</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="19"/>
+                  <c:pt idx="0">
+                    <c:v>6.9376115320008271E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.0147067334188125E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.4286002694185914E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1.9048003592247886E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2.4675822835412031E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>3.1021034421660845E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>3.8776293027076048E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>4.5239008531588727E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>5.4286810237906471E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>6.031867804211831E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>6.7858512797383086E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>7.7552586054152096E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>9.0478017063177455E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>1.0857362047581294E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>1.0857362047581294E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>1.2063735608423662E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>1.3571702559476617E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>1.3571702559476617E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>1.8095603412635491E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>'Varrimento Inicial '!$H$9:$H$27</c:f>
@@ -11411,6 +12263,308 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Varrimento Inicial '!$I$36:$I$54</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="19"/>
+                  <c:pt idx="0">
+                    <c:v>1.0857362047581294E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.6858896380650357E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>7.2382413650541968E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>6.204206884332169E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>5.4286810237906471E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4.8254942433694642E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4.3429448190325179E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>3.9481316536659248E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>3.6191206825270984E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>3.3407267838711675E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>3.1021034421660845E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>2.8952965460216784E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>2.7143405118953235E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>2.5546734229603049E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>2.4127471216847321E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>2.2857604310697464E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>2.1714724095162589E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>2.0680689614440562E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>1.9740658268329624E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Varrimento Inicial '!$I$36:$I$54</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="19"/>
+                  <c:pt idx="0">
+                    <c:v>1.0857362047581294E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.6858896380650357E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>7.2382413650541968E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>6.204206884332169E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>5.4286810237906471E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4.8254942433694642E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4.3429448190325179E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>3.9481316536659248E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>3.6191206825270984E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>3.3407267838711675E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>3.1021034421660845E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>2.8952965460216784E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>2.7143405118953235E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>2.5546734229603049E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>2.4127471216847321E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>2.2857604310697464E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>2.1714724095162589E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>2.0680689614440562E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>1.9740658268329624E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Varrimento Inicial '!$K$36:$K$54</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="19"/>
+                  <c:pt idx="0">
+                    <c:v>6.9155172277587864E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.0340344807220281E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.4476482730108392E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1.9388146513538024E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2.4675822835412031E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>3.1021034421660845E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>3.8776293027076048E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>4.5239008531588727E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>5.4286810237906471E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>6.3866835574007607E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>7.2382413650541968E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>8.3518169596779191E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>9.8703291341648122E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>9.8703291341648122E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>1.2063735608423662E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>1.3571702559476617E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>1.3571702559476617E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>1.5510517210830419E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>1.5510517210830419E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Varrimento Inicial '!$K$36:$K$54</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="19"/>
+                  <c:pt idx="0">
+                    <c:v>6.9155172277587864E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.0340344807220281E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.4476482730108392E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1.9388146513538024E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2.4675822835412031E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>3.1021034421660845E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>3.8776293027076048E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>4.5239008531588727E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>5.4286810237906471E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>6.3866835574007607E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>7.2382413650541968E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>8.3518169596779191E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>9.8703291341648122E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>9.8703291341648122E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>1.2063735608423662E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>1.3571702559476617E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>1.3571702559476617E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>1.5510517210830419E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>1.5510517210830419E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>'Varrimento Inicial '!$H$36:$H$54</c:f>
@@ -13745,6 +14899,320 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'P = K'' d^-2'!$H$9:$H$28</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="20"/>
+                  <c:pt idx="0">
+                    <c:v>1.0093387621558036E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>9.3831699848045567E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>8.7229265599280065E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>8.109140929250929E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>7.5385441065773848E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>7.0080971267645967E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>6.5149748603731967E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>6.056550967193879E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>5.6303839085137879E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>5.2342039436248334E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>4.865901041318072E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>4.5235136419815002E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>4.2052182104488403E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>3.9093195239584238E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>3.6342416434963817E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>3.3785195204380925E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>3.1407911937852973E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>2.9197905364418712E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>2.7143405118953235E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>2.5233469053895089E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'P = K'' d^-2'!$H$9:$H$28</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="20"/>
+                  <c:pt idx="0">
+                    <c:v>1.0093387621558036E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>9.3831699848045567E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>8.7229265599280065E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>8.109140929250929E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>7.5385441065773848E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>7.0080971267645967E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>6.5149748603731967E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>6.056550967193879E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>5.6303839085137879E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>5.2342039436248334E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>4.865901041318072E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>4.5235136419815002E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>4.2052182104488403E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>3.9093195239584238E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>3.6342416434963817E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>3.3785195204380925E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>3.1407911937852973E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>2.9197905364418712E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>2.7143405118953235E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>2.5233469053895089E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'P = K'' d^-2'!$J$9:$J$28</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="20"/>
+                  <c:pt idx="0">
+                    <c:v>7.7002567713342515E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.6858896380650357E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>9.9608826124599026E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1.1309752132897182E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1.2773367114801525E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1.4873098695316844E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1.6964628199345771E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1.9388146513538024E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>2.2157881729757743E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>2.5850862018050701E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>2.8572005388371828E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>3.3929256398691543E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>3.8776293027076048E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>4.3429448190325179E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>4.9351645670824061E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>5.7144010776743657E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>6.7858512797383086E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>7.6325919490905414E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>9.0478017063177455E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>9.8703291341648122E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'P = K'' d^-2'!$J$9:$J$28</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="20"/>
+                  <c:pt idx="0">
+                    <c:v>7.7002567713342515E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.6858896380650357E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>9.9608826124599026E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1.1309752132897182E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1.2773367114801525E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1.4873098695316844E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1.6964628199345771E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1.9388146513538024E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>2.2157881729757743E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>2.5850862018050701E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>2.8572005388371828E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>3.3929256398691543E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>3.8776293027076048E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>4.3429448190325179E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>4.9351645670824061E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>5.7144010776743657E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>6.7858512797383086E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>7.6325919490905414E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>9.0478017063177455E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>9.8703291341648122E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>'P = K'' d^-2'!$G$9:$G$28</c:f>
@@ -25841,8 +27309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AE71A59-C38C-4950-ABA3-969C97DFD363}">
   <dimension ref="B2:Y68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+    <sheetView topLeftCell="B3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U30" sqref="U30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -28063,8 +29531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D17D8F16-3380-4BBB-8E23-4A4730D80727}">
   <dimension ref="A2:AD78"/>
   <sheetViews>
-    <sheetView topLeftCell="I15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView topLeftCell="F4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="V32" sqref="V32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -29785,8 +31253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFAA95BE-4EC9-40BA-AB58-7897911D3F87}">
   <dimension ref="B2:M28"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+    <sheetView topLeftCell="I6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="W33" sqref="W33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -30359,8 +31827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A8E40E-1154-479A-AAB0-0FC0A58E6C1C}">
   <dimension ref="B2:M28"/>
   <sheetViews>
-    <sheetView topLeftCell="H9" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="S32" sqref="S32"/>
+    <sheetView topLeftCell="K6" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="Z22" sqref="Z22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -30937,8 +32405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DCA740D-C390-4794-91E1-ECED3CAE2903}">
   <dimension ref="B2:M28"/>
   <sheetViews>
-    <sheetView topLeftCell="H13" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView topLeftCell="N13" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="Y32" sqref="Y32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -31517,8 +32985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75B9CA03-1F6F-4BA1-96FF-71CF6360130C}">
   <dimension ref="B2:M33"/>
   <sheetViews>
-    <sheetView topLeftCell="G10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView topLeftCell="K7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="Z28" sqref="Z28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -32102,8 +33570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14A442C2-5285-48A4-883D-9C894AAF0160}">
   <dimension ref="B2:U28"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>

</xml_diff>